<commit_message>
stepdefination and exceldata reading is done
</commit_message>
<xml_diff>
--- a/zoebetaBDDFramework/resources-testdata/MyTestdata.xlsx
+++ b/zoebetaBDDFramework/resources-testdata/MyTestdata.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12855" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16005" windowHeight="4245"/>
   </bookViews>
   <sheets>
-    <sheet name="loginpage" sheetId="1" r:id="rId1"/>
+    <sheet name="LOGIN" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:M12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -46,9 +46,6 @@
     <t>anil</t>
   </si>
   <si>
-    <t>shashi</t>
-  </si>
-  <si>
     <t>TestCase_001</t>
   </si>
   <si>
@@ -79,17 +76,29 @@
     <t>TestCase_010</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>prathap@steedserv.com</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>prathap2@steedserv.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +113,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -129,10 +145,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,8 +160,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,13 +460,14 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1">
@@ -476,11 +500,17 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -488,9 +518,15 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -499,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -510,81 +546,85 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="256" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -592,7 +632,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>